<commit_message>
Added memory use to spreadsheet and slides. Added javadoc to ClassDataSharing.
</commit_message>
<xml_diff>
--- a/jlink/Helidon-JRE-Comparisons.xlsx
+++ b/jlink/Helidon-JRE-Comparisons.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
-  <si>
-    <t>Disk Size (MB)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t xml:space="preserve">helidon-se </t>
   </si>
@@ -142,6 +139,18 @@
       </rPr>
       <t xml:space="preserve">CDS archives contain ~ 2500 classes for SE, ~ 5300 for MP </t>
     </r>
+  </si>
+  <si>
+    <t>Memory (kb)</t>
+  </si>
+  <si>
+    <t>Memory (MB)</t>
+  </si>
+  <si>
+    <t>Mem (MB)</t>
+  </si>
+  <si>
+    <t>Disk (MB)</t>
   </si>
 </sst>
 </file>
@@ -580,329 +589,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="2.1640625" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.1640625" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="H2"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="I2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="13">
         <v>1.0049999999999999</v>
       </c>
       <c r="C3" s="14">
+        <f>J3</f>
+        <v>87.846093749999994</v>
+      </c>
+      <c r="D3" s="14">
         <f>279-74+8.6</f>
         <v>213.6</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E3" s="12"/>
+      <c r="F3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>89954.4</v>
+      </c>
+      <c r="J3" s="2">
+        <f>I3/1024</f>
+        <v>87.846093749999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="13">
         <v>0.61899999999999999</v>
       </c>
       <c r="C4" s="14">
+        <f t="shared" ref="C4:C8" si="0">J4</f>
+        <v>87.143749999999997</v>
+      </c>
+      <c r="D4" s="14">
         <f>279-74+8.6+33</f>
         <v>246.6</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E4" s="12"/>
+      <c r="F4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <v>89235.199999999997</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J8" si="1">I4/1024</f>
+        <v>87.143749999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="17">
         <v>1.0069999999999999</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
+        <f t="shared" si="0"/>
+        <v>93.048437500000006</v>
+      </c>
+      <c r="D5" s="18">
         <f>85-32</f>
         <v>53</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E5" s="16"/>
+      <c r="F5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>95281.600000000006</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>93.048437500000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="17">
         <v>0.57199999999999995</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
+        <f t="shared" si="0"/>
+        <v>84.817968750000006</v>
+      </c>
+      <c r="D6" s="18">
         <v>85</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E6" s="16"/>
+      <c r="F6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <v>86853.6</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>84.817968750000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="13">
         <v>0.92400000000000004</v>
       </c>
       <c r="C7" s="14">
+        <f t="shared" si="0"/>
+        <v>88.520312500000003</v>
+      </c>
+      <c r="D7" s="14">
         <f>85-32</f>
         <v>53</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E7" s="12"/>
+      <c r="F7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7">
+        <v>90644.800000000003</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>88.520312500000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="13">
         <v>0.51900000000000002</v>
       </c>
       <c r="C8" s="14">
+        <f t="shared" si="0"/>
+        <v>82.024218750000003</v>
+      </c>
+      <c r="D8" s="14">
         <v>85</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E8" s="12"/>
+      <c r="F8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>83992.8</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>82.024218750000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="D9" s="14"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="13">
         <v>2.9950000000000001</v>
       </c>
       <c r="C10" s="14">
+        <f t="shared" ref="C10:C15" si="2">J10</f>
+        <v>216.62187499999999</v>
+      </c>
+      <c r="D10" s="14">
         <f>279-74+20</f>
         <v>225</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E10" s="12"/>
+      <c r="F10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10">
+        <v>221820.79999999999</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" ref="J10:J15" si="3">I10/1024</f>
+        <v>216.62187499999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="13">
         <v>2.1179999999999999</v>
       </c>
       <c r="C11" s="14">
+        <f t="shared" si="2"/>
+        <v>190.48671874999999</v>
+      </c>
+      <c r="D11" s="14">
         <f>279-74+20+60</f>
         <v>285</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E11" s="12"/>
+      <c r="F11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11">
+        <v>195058.4</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="3"/>
+        <v>190.48671874999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="17">
         <v>3.0310000000000001</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="14">
+        <f t="shared" si="2"/>
+        <v>217.75937500000001</v>
+      </c>
+      <c r="D12" s="18">
         <f>126-60</f>
         <v>66</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E12" s="16"/>
+      <c r="F12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>222985.60000000001</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="3"/>
+        <v>217.75937500000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="17">
         <v>2.093</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="14">
+        <f t="shared" si="2"/>
+        <v>193.03828125000001</v>
+      </c>
+      <c r="D13" s="18">
         <v>126</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E13" s="16"/>
+      <c r="F13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13">
+        <v>197671.2</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="3"/>
+        <v>193.03828125000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="13">
         <v>2.6909999999999998</v>
       </c>
       <c r="C14" s="14">
+        <f t="shared" si="2"/>
+        <v>194.99765625000001</v>
+      </c>
+      <c r="D14" s="14">
         <f>124-60</f>
         <v>64</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="E14" s="12"/>
+      <c r="F14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>199677.6</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="3"/>
+        <v>194.99765625000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="13">
         <v>1.93</v>
       </c>
       <c r="C15" s="14">
+        <f t="shared" si="2"/>
+        <v>192.32421875</v>
+      </c>
+      <c r="D15" s="14">
         <f>124</f>
         <v>124</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E15" s="12"/>
+      <c r="F15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>196940</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="3"/>
+        <v>192.32421875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added slide to deck. Added missing javadoc to JarsLinker classes.
</commit_message>
<xml_diff>
--- a/jlink/Helidon-JRE-Comparisons.xlsx
+++ b/jlink/Helidon-JRE-Comparisons.xlsx
@@ -251,8 +251,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -303,17 +305,19 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -592,7 +596,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>